<commit_message>
rev 3 update w. new mechanical and update on HW
</commit_message>
<xml_diff>
--- a/Hardware/Mainboard/production/BOM1.xlsx
+++ b/Hardware/Mainboard/production/BOM1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/891171bab38366e0/Dokumenter/GitHub/BeeSMART/Hardware/Mainboard/production/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/891171bab38366e0/Stuff/Projekter/DosingESP32/Hardware/mainboard/Assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="353" documentId="13_ncr:1_{55000A20-6122-4704-9F23-9D02A4D9B46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81F08660-6E67-4660-A6E2-A8297BDBBD39}"/>
+  <xr:revisionPtr revIDLastSave="352" documentId="13_ncr:1_{55000A20-6122-4704-9F23-9D02A4D9B46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F369540F-0E25-443A-968B-18A481C12A90}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{F2DF9297-AA5E-464F-BE05-B9D32E6A1A51}"/>
+    <workbookView xWindow="12900" yWindow="3375" windowWidth="38700" windowHeight="15345" xr2:uid="{F2DF9297-AA5E-464F-BE05-B9D32E6A1A51}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,7 +205,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,6 +229,17 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -249,7 +260,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -273,6 +284,47 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color rgb="FF3F3F3F"/>
@@ -286,7 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1"/>
@@ -296,10 +348,23 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,13 +680,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25290214-CED8-4CB3-BC64-B0DDC2AA47C8}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
@@ -629,7 +694,7 @@
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -643,7 +708,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
@@ -656,8 +721,11 @@
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>40</v>
       </c>
@@ -670,8 +738,11 @@
       <c r="D3" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="7"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
         <v>47</v>
       </c>
@@ -684,8 +755,11 @@
       <c r="D4" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -698,8 +772,11 @@
       <c r="D5" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -712,8 +789,11 @@
       <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -726,8 +806,11 @@
       <c r="D7" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -740,8 +823,11 @@
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -754,8 +840,11 @@
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="4" t="s">
         <v>21</v>
       </c>
@@ -768,8 +857,11 @@
       <c r="D10" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="7"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="4" t="s">
         <v>34</v>
       </c>
@@ -782,8 +874,9 @@
       <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="6"/>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>27</v>
       </c>
@@ -796,8 +889,9 @@
       <c r="D12" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>28</v>
       </c>
@@ -810,8 +904,9 @@
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="11"/>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -824,18 +919,19 @@
       <c r="D14" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="6"/>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>50</v>
       </c>
       <c r="B15" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="10" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>